<commit_message>
test some m4 barrel/ammo changes
</commit_message>
<xml_diff>
--- a/changes/m4-barrels.xlsx
+++ b/changes/m4-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EAF93A-40F6-4DFD-A187-DB46DF15B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F9087-C9C0-4B2D-BEA2-29A5BD746BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,10 +1017,13 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
@@ -1111,6 +1114,9 @@
       <c r="J3">
         <v>550</v>
       </c>
+      <c r="L3">
+        <v>-0.05</v>
+      </c>
       <c r="M3">
         <v>5000</v>
       </c>
@@ -1167,6 +1173,9 @@
       <c r="J4">
         <v>367</v>
       </c>
+      <c r="L4">
+        <v>-0.05</v>
+      </c>
       <c r="M4">
         <v>1600</v>
       </c>
@@ -1220,6 +1229,9 @@
       <c r="J5">
         <v>379</v>
       </c>
+      <c r="L5">
+        <v>-0.05</v>
+      </c>
       <c r="M5">
         <v>2000</v>
       </c>
@@ -1276,6 +1288,9 @@
       <c r="J6">
         <v>267</v>
       </c>
+      <c r="L6">
+        <v>-0.02</v>
+      </c>
       <c r="M6">
         <v>1800</v>
       </c>
@@ -1332,6 +1347,9 @@
       <c r="J7">
         <v>178</v>
       </c>
+      <c r="L7">
+        <v>-0.02</v>
+      </c>
       <c r="M7">
         <v>1100</v>
       </c>
@@ -1374,7 +1392,7 @@
         <v>0.72</v>
       </c>
       <c r="E8">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="F8">
         <v>-6</v>
@@ -1393,7 +1411,7 @@
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>-7.1049999999999978</v>
+        <v>-7.9049999999999985</v>
       </c>
       <c r="P8">
         <v>0.04</v>
@@ -1720,6 +1738,9 @@
       </c>
       <c r="J14">
         <v>-633</v>
+      </c>
+      <c r="L14">
+        <v>0.03</v>
       </c>
       <c r="M14">
         <v>1300</v>

</xml_diff>

<commit_message>
adjust aug barrel damage and fix m4 firerates
</commit_message>
<xml_diff>
--- a/changes/m4-barrels.xlsx
+++ b/changes/m4-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F9087-C9C0-4B2D-BEA2-29A5BD746BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9A6A531-5309-4D2E-BB3B-5866F69004AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,20 +1109,20 @@
         <v>-0.3</v>
       </c>
       <c r="I3">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="J3">
         <v>550</v>
       </c>
       <c r="L3">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="M3">
         <v>5000</v>
       </c>
       <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/200</f>
-        <v>-8.6500000000000021</v>
+        <v>-9.1500000000000021</v>
       </c>
       <c r="P3">
         <v>0.08</v>
@@ -1168,20 +1168,20 @@
         <v>-0.2</v>
       </c>
       <c r="I4">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="J4">
         <v>367</v>
       </c>
       <c r="L4">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="M4">
         <v>1600</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N16" si="1">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*5+J4/200</f>
-        <v>-8.2650000000000006</v>
+        <v>-8.4649999999999999</v>
       </c>
       <c r="P4">
         <v>0.08</v>
@@ -1224,20 +1224,20 @@
         <v>-0.22</v>
       </c>
       <c r="I5">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="J5">
         <v>379</v>
       </c>
       <c r="L5">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="M5">
         <v>2000</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>-8.3049999999999979</v>
+        <v>-8.5049999999999972</v>
       </c>
       <c r="P5">
         <v>0.08</v>
@@ -1268,7 +1268,7 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="D6">
         <v>0.74</v>
@@ -1283,20 +1283,20 @@
         <v>-0.1</v>
       </c>
       <c r="I6">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="J6">
         <v>267</v>
       </c>
       <c r="L6">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="M6">
         <v>1800</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>-7.7650000000000015</v>
+        <v>-6.9650000000000007</v>
       </c>
       <c r="P6">
         <v>0.06</v>
@@ -1345,17 +1345,17 @@
         <v>0.1</v>
       </c>
       <c r="J7">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="L7">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="M7">
         <v>1100</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>-6.81</v>
+        <v>-6.9999999999999991</v>
       </c>
       <c r="P7">
         <v>0.06</v>
@@ -1404,14 +1404,14 @@
         <v>0.12</v>
       </c>
       <c r="J8">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="M8">
         <v>1200</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>-7.9049999999999985</v>
+        <v>-7.6499999999999986</v>
       </c>
       <c r="P8">
         <v>0.04</v>
@@ -1460,14 +1460,14 @@
         <v>0.04</v>
       </c>
       <c r="J9">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="M9">
         <v>800</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>-7.0850000000000009</v>
+        <v>-7.2000000000000011</v>
       </c>
       <c r="P9">
         <v>0.04</v>
@@ -1516,14 +1516,14 @@
         <v>0.02</v>
       </c>
       <c r="J10">
-        <v>-22</v>
+        <v>-10</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
-        <v>-7.21</v>
+        <v>-7.1499999999999995</v>
       </c>
       <c r="P10">
         <v>0.04</v>

</xml_diff>